<commit_message>
new form field and edit functionlaity
</commit_message>
<xml_diff>
--- a/backend/income_details.xlsx
+++ b/backend/income_details.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -413,27 +413,36 @@
       <c r="C1" t="str">
         <v>Date</v>
       </c>
+      <c r="D1" t="str">
+        <v>Notes</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Trading Profit</v>
+        <v>pppp</v>
       </c>
       <c r="B2">
-        <v>15000</v>
+        <v>5000</v>
       </c>
       <c r="C2" s="1">
-        <v>45785.23976851852</v>
+        <v>45982.23976851852</v>
+      </c>
+      <c r="D2" t="str">
+        <v>helooiii</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Interest From Saving Account</v>
+        <v>Salary</v>
       </c>
       <c r="B3">
-        <v>4500</v>
+        <v>25000</v>
       </c>
       <c r="C3" s="1">
-        <v>45781.23976851852</v>
+        <v>45966.23976851852</v>
+      </c>
+      <c r="D3" t="str">
+        <v/>
       </c>
     </row>
     <row r="4">
@@ -441,15 +450,144 @@
         <v>Salary</v>
       </c>
       <c r="B4">
-        <v>35000</v>
+        <v>5000</v>
       </c>
       <c r="C4" s="1">
-        <v>45778.23976851852</v>
+        <v>45966.23976851852</v>
+      </c>
+      <c r="D4" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>Salary2</v>
+      </c>
+      <c r="B5">
+        <v>50000</v>
+      </c>
+      <c r="C5" s="1">
+        <v>45966.23976851852</v>
+      </c>
+      <c r="D5" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>random</v>
+      </c>
+      <c r="B6">
+        <v>234345</v>
+      </c>
+      <c r="C6" s="1">
+        <v>45966.23976851852</v>
+      </c>
+      <c r="D6" t="str">
+        <v>yoyoyo</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>fsdfvds</v>
+      </c>
+      <c r="B7">
+        <v>12345</v>
+      </c>
+      <c r="C7" s="1">
+        <v>45926.23976851852</v>
+      </c>
+      <c r="D7" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>salary2</v>
+      </c>
+      <c r="B8">
+        <v>25367</v>
+      </c>
+      <c r="C8" s="1">
+        <v>45925.23976851852</v>
+      </c>
+      <c r="D8" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>Interest</v>
+      </c>
+      <c r="B9">
+        <v>50000</v>
+      </c>
+      <c r="C9" s="1">
+        <v>45922.23976851852</v>
+      </c>
+      <c r="D9" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>utilities</v>
+      </c>
+      <c r="B10">
+        <v>2386</v>
+      </c>
+      <c r="C10" s="1">
+        <v>45905.23976851852</v>
+      </c>
+      <c r="D10" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>salary</v>
+      </c>
+      <c r="B11">
+        <v>50000</v>
+      </c>
+      <c r="C11" s="1">
+        <v>45904.23976851852</v>
+      </c>
+      <c r="D11" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>salary1</v>
+      </c>
+      <c r="B12">
+        <v>50000</v>
+      </c>
+      <c r="C12" s="1">
+        <v>45904.23976851852</v>
+      </c>
+      <c r="D12" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>salary</v>
+      </c>
+      <c r="B13">
+        <v>50000</v>
+      </c>
+      <c r="C13" s="1">
+        <v>45870.23976851852</v>
+      </c>
+      <c r="D13" t="str">
+        <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D13"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>